<commit_message>
Corrigido localização do Keys.
</commit_message>
<xml_diff>
--- a/date.xlsx
+++ b/date.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeuge\PycharmProjects\autozap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA6661A-69F9-42BB-837A-099D10604B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA472E3-F0E8-4ECD-B878-4D1BB5752F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1D3A1140-D5BB-4095-89C1-2941E6CBC8FF}"/>
+    <workbookView xWindow="20370" yWindow="-4665" windowWidth="29040" windowHeight="15840" xr2:uid="{1D3A1140-D5BB-4095-89C1-2941E6CBC8FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Ana</t>
   </si>
   <si>
-    <t>Nós do @merendinhajf gostariámos de conhecer melhor você e seu pequeno(a). Preencha o formulario pelo link abaixo para nos ajudar a cada vez mais atende-los melhor.</t>
-  </si>
-  <si>
     <t>Junior</t>
   </si>
   <si>
@@ -55,15 +52,24 @@
   <si>
     <t>numero</t>
   </si>
+  <si>
+    <t>Nós do @merendinhajf gostariámos de conhecer melhor você e seu pequeno(a). Preencha o formulario pelo link abaixo para nos ajudar a cada vez mais atende-los melhor.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -414,27 +420,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B861025-D833-48EF-B934-8AD29412E61E}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="53.28515625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -451,7 +457,7 @@
         <v>5532987105144</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -459,16 +465,29 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>5531991534878</v>
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5532991170287</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Corrigido integração com o Chrome
</commit_message>
<xml_diff>
--- a/date.xlsx
+++ b/date.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeuge\PycharmProjects\autozap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CA5233-65F9-4401-9684-9BF42BF631A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EA38E1-23B0-4F43-8AEF-2127D764507E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4665" windowWidth="29040" windowHeight="15840" xr2:uid="{1D3A1140-D5BB-4095-89C1-2941E6CBC8FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="18015" windowHeight="11040" xr2:uid="{1D3A1140-D5BB-4095-89C1-2941E6CBC8FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -23,23 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
-  <si>
-    <t>mensagem</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Ana</t>
   </si>
@@ -56,22 +45,19 @@
     <t>Isis</t>
   </si>
   <si>
-    <t>Viviane</t>
-  </si>
-  <si>
-    <t>Renata</t>
-  </si>
-  <si>
-    <t>Alessandra</t>
-  </si>
-  <si>
-    <t>Nós do @merendinhajf gostariámos de conhecer melhor você e seu pequeno(a). Preencha o formulario pelo link abaixo para nos ajudar a cada vez mais atende-los melhor.  **Mensagem teste do BOT Automaizador de envio de mensagens no Whatsapp**</t>
+    <t>valor</t>
+  </si>
+  <si>
+    <t>Manuela</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,10 +98,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -432,114 +418,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B861025-D833-48EF-B934-8AD29412E61E}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="53.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" style="3" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
         <v>5532987105144</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
+      <c r="D2" s="3">
+        <v>37.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
         <v>5532991170287</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
+      <c r="D3" s="3">
+        <v>122.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
         <v>5532988329968</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
+      <c r="D4" s="3">
+        <v>200.2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
-        <v>5532988090045</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3">
-        <v>5532988154186</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3">
-        <v>5532988220411</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
+      <c r="C5" s="2">
+        <v>5532991599484</v>
+      </c>
+      <c r="D5" s="3">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>